<commit_message>
Fragen "Aeltere Arbeitnehmende": Diverse kleine Verbesserungen, BUGFIX: Alle Fragen und Antworten mit Kindern ersetzt.
</commit_message>
<xml_diff>
--- a/inst/shiny-apps/vsim/data/vsim_question_lists_aeltere_arbeitnehmende.xlsx
+++ b/inst/shiny-apps/vsim/data/vsim_question_lists_aeltere_arbeitnehmende.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianschmid/Documents/R/vsim/inst/shiny-apps/vsim/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2204DA87-83C3-044C-84CD-42B9906B9308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819DCC46-639E-C24A-8691-8E0FE46D1A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
   </bookViews>
   <sheets>
     <sheet name="QAGlist_Teil1" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Qlist_Teil2c" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_4" localSheetId="0" hidden="1">QAGlist_Teil1!$A$1:$G$31</definedName>
+    <definedName name="ExterneDaten_4" localSheetId="0" hidden="1">QAGlist_Teil1!$A$1:$G$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="144">
   <si>
     <t>Qnum</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Unzufriedenheit mit dem privaten Zeitmanagement</t>
   </si>
   <si>
-    <t>Unzufriedenheit mit der zeitlichen Organisation der Kinderbetreuung</t>
-  </si>
-  <si>
     <t>Vereinbarkeitstätigkeit Switchen wird angewandt</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t>für Hausarbeiten</t>
   </si>
   <si>
-    <t>für Kinderbetreuung</t>
-  </si>
-  <si>
     <t>für soziale Kontakte</t>
   </si>
   <si>
@@ -287,33 +281,12 @@
     <t>Ja, ich möchte gerne aushandeln, dass ich einen grösseren Teil und meine Angehörigen einen kleineren Teil beitragen</t>
   </si>
   <si>
-    <t>Möchten Sie einplanen, dass Ihre Kinder neu oder in einem anderen Umfang als bisher durch Grosseltern, andere Verwandte, Freunde oder Nachbarn betreut werden?</t>
-  </si>
-  <si>
-    <t>Ja, ich möchte mehr Unterstützung bei der Kinderbetreuung einplanen</t>
-  </si>
-  <si>
-    <t>Ja, ich möchte die Kinder mehr selbst betreuen als bisher</t>
-  </si>
-  <si>
     <t>Nein, ich möchte diese Massnahme nicht einplanen</t>
   </si>
   <si>
     <t>Nein, in unserem Umfeld kommt niemand in Frage</t>
   </si>
   <si>
-    <t>Möchten Sie einplanen, dass Ihre Kinder neu oder in einem anderen Umfang als bisher durch Krippen, Tagesschulen, Spielgruppen oder ähnliche Organisationen betreut werden?</t>
-  </si>
-  <si>
-    <t>Ja, ich möchte mehr Unterstützung bei der Kinderbetreuung einplanen als bisher</t>
-  </si>
-  <si>
-    <t>Ja, ich möchte die Kinder mehr selbst betreuen als bisher, um Geld zu sparen</t>
-  </si>
-  <si>
-    <t>Ja, ich möchte die Kinder mehr selbst betreuen als bisher, um mehr Zeit mit ihnen zu verbringen</t>
-  </si>
-  <si>
     <t>Möchten Sie einplanen, Hausarbeiten in einem anderen Umfang als bisher an bezahlte Drittpersonen auszulagern (z.B. Haushaltshilfe, Gärtner, Essen bestellen)?</t>
   </si>
   <si>
@@ -419,9 +392,6 @@
     <t>Arbeit,Haushalt &amp; Selbstsorge</t>
   </si>
   <si>
-    <t>Ich fühle mich in meiner Arbeit wertgeschätzt durch meine Kolleg_innen, Vorgesetzten und die Firmenleitung</t>
-  </si>
-  <si>
     <t>Ich bin zufrieden mit meinen aktuellen Möglichkeiten zur Karriereentwicklung.</t>
   </si>
   <si>
@@ -437,12 +407,6 @@
     <t>Ich fühle mich belastet, weil ich während der Arbeit oft auch privaten Verpflichtungen nachkommen muss</t>
   </si>
   <si>
-    <t xml:space="preserve">Ich fühle mich belastet, weil ich zu Hause oft auch beruflichen Verpflichtungen nachkommen muss.  </t>
-  </si>
-  <si>
-    <t>Ich fühle mich belastet, weil ich ausserhalb meiner Arbeitszeit oft auch beruflichen Verpflichtungen nachkommen muss und deshalb zu wenig Zeit für andere Tätigkeiten habe.</t>
-  </si>
-  <si>
     <t>Ich fühle mich während des Home Office belastet, weil oft private Aufgaben dazwischen kommen.</t>
   </si>
   <si>
@@ -479,10 +443,34 @@
     <t xml:space="preserve">Ich habe ein schlechtes Gewissen, weil ich aufgrund von beruflichen Verpflichtungen meine Erwartungen bezüglich Haushalt oder der Betreuung von Angehörigen nicht erfüllen kann.  </t>
   </si>
   <si>
-    <t>Ich fühle mich oft durch die Gedanken an meine Pensionierung aus finanziellen, sozialen (Verlust von Arbeitsumfeld) oder anderen Gründen belastet.</t>
-  </si>
-  <si>
     <t>Belastung: Pensionierung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich fühle mich belastet, weil ich ausserhalb meiner Arbeitszeit oft auch beruflichen Verpflichtungen nachkommen muss.  </t>
+  </si>
+  <si>
+    <t>Unzufriedenheit mit der zeitlichen Organisation der Betreuung von Angehörigen</t>
+  </si>
+  <si>
+    <t>Ich fühle mich in meiner Arbeit wertgeschätzt durch meine Kolleg_innen, Vorgesetzten und die Firmenleitung.</t>
+  </si>
+  <si>
+    <t>Ich fühle mich durch die Gedanken an meine Pensionierung aus finanziellen, sozialen (Verlust von Arbeitsumfeld) oder anderen Gründen belastet.</t>
+  </si>
+  <si>
+    <t>für Betreuung von Angehörigen</t>
+  </si>
+  <si>
+    <t>Möchten Sie einplanen, dass Ihre Angehörigen neu oder in einem anderen Umfang als bisher durch andere Verwandte, Freunde oder Nachbarn betreut werden?</t>
+  </si>
+  <si>
+    <t>Möchten Sie einplanen, dass Ihre Angehörigen neu oder in einem anderen Umfang als bisher professionell betreut werden?</t>
+  </si>
+  <si>
+    <t>Ja, ich möchte mehr Unterstützung einplanen</t>
+  </si>
+  <si>
+    <t>Ja, ich möchte mehr Betreuungsaufgaben übernehmen</t>
   </si>
 </sst>
 </file>
@@ -723,8 +711,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9A4626D1-B7A1-4A0E-9ABD-F1802EEF4B4A}" name="Qlist_Teil1" displayName="Qlist_Teil1" ref="A1:M31" totalsRowShown="0">
-  <autoFilter ref="A1:M31" xr:uid="{63A3C723-9C80-47B3-B07E-C2015D435A2D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9A4626D1-B7A1-4A0E-9ABD-F1802EEF4B4A}" name="Qlist_Teil1" displayName="Qlist_Teil1" ref="A1:M30" totalsRowShown="0">
+  <autoFilter ref="A1:M30" xr:uid="{63A3C723-9C80-47B3-B07E-C2015D435A2D}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{6833DAB1-3042-428C-936F-D4BF6D9DD972}" name="Qnum" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{68ACE6E4-2458-484E-B5F0-6043D861F09A}" name="Question" dataDxfId="21"/>
@@ -1081,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F2727F-E159-4B39-B30A-A10ACC8F5533}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1111,22 +1099,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -1141,22 +1129,22 @@
         <v>9</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1174,22 +1162,22 @@
         <v>12</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
@@ -1209,22 +1197,22 @@
         <v>12</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
@@ -1232,7 +1220,7 @@
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>11</v>
@@ -1244,7 +1232,7 @@
         <v>12</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1253,27 +1241,27 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="K5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1281,7 +1269,7 @@
         <v>12</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1290,27 +1278,27 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="K6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1318,35 +1306,35 @@
         <v>12</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>12</v>
@@ -1355,35 +1343,35 @@
         <v>12</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>12</v>
@@ -1392,22 +1380,22 @@
         <v>12</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
@@ -1415,10 +1403,10 @@
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>12</v>
@@ -1431,16 +1419,16 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
@@ -1448,10 +1436,10 @@
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>12</v>
@@ -1464,16 +1452,16 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
@@ -1481,10 +1469,10 @@
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>12</v>
@@ -1497,122 +1485,122 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="8"/>
       <c r="I12" s="5" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="8"/>
       <c r="I13" s="5" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="8"/>
       <c r="I14" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K15" s="5" t="s">
         <v>12</v>
@@ -1621,7 +1609,7 @@
         <v>12</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1630,26 +1618,26 @@
         <v>3</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K16" s="5" t="s">
         <v>12</v>
@@ -1658,35 +1646,35 @@
         <v>12</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>12</v>
@@ -1695,35 +1683,35 @@
         <v>12</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>12</v>
@@ -1732,35 +1720,35 @@
         <v>12</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>12</v>
@@ -1769,35 +1757,35 @@
         <v>12</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>12</v>
@@ -1806,35 +1794,35 @@
         <v>12</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>12</v>
@@ -1843,36 +1831,36 @@
         <v>12</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="K22" s="5" t="s">
         <v>12</v>
       </c>
@@ -1880,35 +1868,35 @@
         <v>12</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>12</v>
@@ -1917,103 +1905,103 @@
         <v>12</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="G24" s="3"/>
       <c r="H24" s="8"/>
       <c r="I24" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
       <c r="M24" s="6" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="H25" s="8"/>
       <c r="I25" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="M25" s="6" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="5" t="s">
-        <v>31</v>
+        <v>134</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>12</v>
@@ -2022,35 +2010,35 @@
         <v>12</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="5" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>12</v>
@@ -2059,35 +2047,35 @@
         <v>12</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="5" t="s">
-        <v>120</v>
+        <v>31</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>12</v>
@@ -2096,25 +2084,25 @@
         <v>12</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>12</v>
@@ -2124,7 +2112,7 @@
         <v>32</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>12</v>
@@ -2133,25 +2121,25 @@
         <v>12</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>12</v>
@@ -2161,7 +2149,7 @@
         <v>33</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>12</v>
@@ -2170,44 +2158,7 @@
         <v>12</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="8"/>
-      <c r="I31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2224,13 +2175,13 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="190.5" customWidth="1"/>
     <col min="3" max="3" width="68.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2243,10 +2194,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2254,10 +2205,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
@@ -2268,10 +2219,10 @@
         <v>1.2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
@@ -2282,10 +2233,10 @@
         <v>2.1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -2296,10 +2247,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
@@ -2310,10 +2261,10 @@
         <v>3.1</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -2324,10 +2275,10 @@
         <v>3.2</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
@@ -2338,10 +2289,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -2352,10 +2303,10 @@
         <v>4.2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
@@ -2366,10 +2317,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
@@ -2380,10 +2331,10 @@
         <v>5.2</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
@@ -2394,10 +2345,10 @@
         <v>6.1</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -2408,10 +2359,10 @@
         <v>6.2</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
@@ -2430,7 +2381,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2452,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2460,7 +2411,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2468,7 +2419,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2476,7 +2427,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2484,7 +2435,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2492,7 +2443,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2510,14 +2461,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E396E85-B3B1-449F-B640-6DB26BD002CF}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118" customWidth="1"/>
     <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="81.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="71.5" bestFit="1" customWidth="1"/>
@@ -2532,19 +2483,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
-      </c>
-      <c r="F1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2552,16 +2503,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
@@ -2575,19 +2526,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>143</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -2598,20 +2549,18 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>85</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2621,19 +2570,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
@@ -2644,16 +2593,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>12</v>
@@ -2667,19 +2616,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
@@ -2690,16 +2639,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>12</v>
@@ -2713,16 +2662,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Fragen (beide Versionen): Antwortkategorien Teil 2c konsistent. Immer zuerst "Nein.."
</commit_message>
<xml_diff>
--- a/inst/shiny-apps/vsim/data/vsim_question_lists_aeltere_arbeitnehmende.xlsx
+++ b/inst/shiny-apps/vsim/data/vsim_question_lists_aeltere_arbeitnehmende.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianschmid/Documents/R/vsim/inst/shiny-apps/vsim/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819DCC46-639E-C24A-8691-8E0FE46D1A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93E8CE6-C9A3-AB4F-859E-90CB202C493A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="143">
   <si>
     <t>Qnum</t>
   </si>
@@ -279,9 +279,6 @@
   </si>
   <si>
     <t>Ja, ich möchte gerne aushandeln, dass ich einen grösseren Teil und meine Angehörigen einen kleineren Teil beitragen</t>
-  </si>
-  <si>
-    <t>Nein, ich möchte diese Massnahme nicht einplanen</t>
   </si>
   <si>
     <t>Nein, in unserem Umfeld kommt niemand in Frage</t>
@@ -1114,7 +1111,7 @@
         <v>66</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -1129,13 +1126,13 @@
         <v>9</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>67</v>
@@ -1162,13 +1159,13 @@
         <v>12</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>67</v>
@@ -1197,13 +1194,13 @@
         <v>12</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>67</v>
@@ -1220,7 +1217,7 @@
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>11</v>
@@ -1232,7 +1229,7 @@
         <v>12</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1269,7 +1266,7 @@
         <v>12</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1306,7 +1303,7 @@
         <v>12</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1343,7 +1340,7 @@
         <v>12</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1380,19 +1377,19 @@
         <v>12</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>69</v>
@@ -1406,7 +1403,7 @@
         <v>14</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>12</v>
@@ -1422,10 +1419,10 @@
         <v>70</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>69</v>
@@ -1439,7 +1436,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>12</v>
@@ -1452,13 +1449,13 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>69</v>
@@ -1472,7 +1469,7 @@
         <v>16</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>12</v>
@@ -1485,7 +1482,7 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>71</v>
@@ -1502,7 +1499,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="8"/>
       <c r="I12" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>18</v>
@@ -1510,13 +1507,13 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>71</v>
@@ -1533,7 +1530,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="8"/>
       <c r="I13" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>18</v>
@@ -1541,13 +1538,13 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>71</v>
@@ -1564,7 +1561,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="8"/>
       <c r="I14" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>18</v>
@@ -1572,13 +1569,13 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>71</v>
@@ -1609,7 +1606,7 @@
         <v>12</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1646,13 +1643,13 @@
         <v>12</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>71</v>
@@ -1683,13 +1680,13 @@
         <v>12</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>71</v>
@@ -1720,13 +1717,13 @@
         <v>12</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>71</v>
@@ -1757,13 +1754,13 @@
         <v>12</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>71</v>
@@ -1794,13 +1791,13 @@
         <v>12</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>71</v>
@@ -1831,13 +1828,13 @@
         <v>12</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>71</v>
@@ -1868,13 +1865,13 @@
         <v>12</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>71</v>
@@ -1905,13 +1902,13 @@
         <v>12</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>71</v>
@@ -1936,13 +1933,13 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>71</v>
@@ -1973,13 +1970,13 @@
         <v>12</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>71</v>
@@ -1998,7 +1995,7 @@
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>24</v>
@@ -2010,13 +2007,13 @@
         <v>12</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>71</v>
@@ -2035,7 +2032,7 @@
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>24</v>
@@ -2047,13 +2044,13 @@
         <v>12</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>71</v>
@@ -2084,13 +2081,13 @@
         <v>12</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>71</v>
@@ -2121,13 +2118,13 @@
         <v>12</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>71</v>
@@ -2158,7 +2155,7 @@
         <v>12</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2419,7 +2416,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2443,7 +2440,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2462,7 +2459,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2526,19 +2523,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -2549,16 +2546,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
@@ -2570,19 +2567,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
@@ -2593,16 +2590,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>12</v>
@@ -2616,19 +2613,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
@@ -2639,16 +2636,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>12</v>
@@ -2662,16 +2659,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Use of new Gaps from Myriel (new Excels). Everything seems to work fine - new gaps are adopted perfectly.
</commit_message>
<xml_diff>
--- a/inst/shiny-apps/vsim/data/vsim_question_lists_aeltere_arbeitnehmende.xlsx
+++ b/inst/shiny-apps/vsim/data/vsim_question_lists_aeltere_arbeitnehmende.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianschmid/Documents/R/vsim/inst/shiny-apps/vsim/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAY\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93E8CE6-C9A3-AB4F-859E-90CB202C493A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95703483-9EE1-42FA-83BF-D5DF9ABC0B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
   </bookViews>
   <sheets>
     <sheet name="QAGlist_Teil1" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="147">
   <si>
     <t>Qnum</t>
   </si>
@@ -71,18 +71,12 @@
     <t>Indikator2</t>
   </si>
   <si>
-    <t>Unzufriedenheit mit dem beruflichen Zeitmanagement</t>
-  </si>
-  <si>
     <t>Nein, ich möchte gern weniger Zeit dafür verwenden,Nein, ich möchte gern mehr Zeit dafür verwenden</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Unzufriedenheit mit dem privaten Zeitmanagement</t>
-  </si>
-  <si>
     <t>Vereinbarkeitstätigkeit Switchen wird angewandt</t>
   </si>
   <si>
@@ -92,15 +86,9 @@
     <t>Vereinbarkeitstätigkeit Flexible Arbeitszeiten wird angewandt</t>
   </si>
   <si>
-    <t>Unzufriedenheit mit sozialen Beziehungen</t>
-  </si>
-  <si>
     <t>Trifft eher nicht zu,Trifft überhaupt nicht zu</t>
   </si>
   <si>
-    <t>Unzufriedenheit mit der Selbstsorge</t>
-  </si>
-  <si>
     <t>In meiner Freizeit verbringe ich genügend Zeit mit Freunden/Verwandten oder in Vereinen, Sportclubs und/oder Ähnlichem.</t>
   </si>
   <si>
@@ -116,33 +104,15 @@
     <t>Trifft voll und ganz zu,Trifft eher zu</t>
   </si>
   <si>
-    <t>Belastung: Stress im Privaten</t>
-  </si>
-  <si>
-    <t>Belastung: Stress bei der Arbeit</t>
-  </si>
-  <si>
-    <t>Belastung: Viele zeitgleiche Aufgaben (privat und/oder beruflich)</t>
-  </si>
-  <si>
     <t>Belastung: Keine klar festgelegeten Arbeitszeiten (Flexibilisierung)</t>
   </si>
   <si>
     <t>Belastung: Störungen beim Arbeiten im Home Office</t>
   </si>
   <si>
-    <t>Belastung: Hohe zeitliche Beanspruchung</t>
-  </si>
-  <si>
     <t>Belastung: Finanzielle Situation</t>
   </si>
   <si>
-    <t>Belastung: Gesundheitliche Situation</t>
-  </si>
-  <si>
-    <t>Belastung: Psychische oder emotionale Belastung</t>
-  </si>
-  <si>
     <t>Massnahme</t>
   </si>
   <si>
@@ -356,15 +326,9 @@
     <t>Unzufriedenheit mit den Arbeitsinhalten</t>
   </si>
   <si>
-    <t>Unzufriedenheit mit der Wertschätzung</t>
-  </si>
-  <si>
     <t>Ich bin zufrieden mit dem Lohn, den ich für meine Arbeit erhalte.</t>
   </si>
   <si>
-    <t>Unzufriedenheit mit dem Lohn</t>
-  </si>
-  <si>
     <t>Ich fühle mich belastet, weil ich meine Aufgaben bei der Arbeit unter hohem Zeitdruck erledigen muss.</t>
   </si>
   <si>
@@ -398,18 +362,12 @@
     <t>Ich habe ein schlechtes Gewissen, weil ich aufgrund von privaten Verpflichtungen die Erwartungen meines Arbeitgebers und/oder meiner Arbeitskolleg_innen oft nicht erfüllen kann.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ich fühle mich belastet, weil ich während der Arbeit oder in der Freizeit oft verschiedene Dinge gleichzeitig erledigen muss. </t>
-  </si>
-  <si>
     <t>Ich fühle mich belastet, weil ich während der Arbeit oft auch privaten Verpflichtungen nachkommen muss</t>
   </si>
   <si>
     <t>Ich fühle mich während des Home Office belastet, weil oft private Aufgaben dazwischen kommen.</t>
   </si>
   <si>
-    <t>Ich fühle mich belastet, weil die zeitliche Beanspruchung von Arbeit und privaten Verpflichtungen insgesamt zu hoch ist.</t>
-  </si>
-  <si>
     <t>Ich fühle mich belastet, weil die finanzielle Situation in meinem Haushalt angespannt ist.</t>
   </si>
   <si>
@@ -440,15 +398,9 @@
     <t xml:space="preserve">Ich habe ein schlechtes Gewissen, weil ich aufgrund von beruflichen Verpflichtungen meine Erwartungen bezüglich Haushalt oder der Betreuung von Angehörigen nicht erfüllen kann.  </t>
   </si>
   <si>
-    <t>Belastung: Pensionierung</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ich fühle mich belastet, weil ich ausserhalb meiner Arbeitszeit oft auch beruflichen Verpflichtungen nachkommen muss.  </t>
   </si>
   <si>
-    <t>Unzufriedenheit mit der zeitlichen Organisation der Betreuung von Angehörigen</t>
-  </si>
-  <si>
     <t>Ich fühle mich in meiner Arbeit wertgeschätzt durch meine Kolleg_innen, Vorgesetzten und die Firmenleitung.</t>
   </si>
   <si>
@@ -468,6 +420,66 @@
   </si>
   <si>
     <t>Ja, ich möchte mehr Betreuungsaufgaben übernehmen</t>
+  </si>
+  <si>
+    <t>Belastung: Organisierung des Alltags kompliziert</t>
+  </si>
+  <si>
+    <t>Ich fühle mich belastet, weil die Organisierung des Alltags oft kompliziert ist (z.B. Administration/Pflege von Angehörigen erledigen, Hausarbeiten, Einkäufe etc.)</t>
+  </si>
+  <si>
+    <t>Belastung: Gedanken an Pensionierung</t>
+  </si>
+  <si>
+    <t>Belastung: Psychische Gesundheit</t>
+  </si>
+  <si>
+    <t>Belastung: Körperliche Gesundheit</t>
+  </si>
+  <si>
+    <t>Ich fühle mich bei der Unterstützung von Angehörigen belastet, da ich das Gefühl habe, zunehmend mehr Zeit und Energie darauf verwenden zu müssen.</t>
+  </si>
+  <si>
+    <t>Belastung: Zunehmender Unterstützungsbedarf Angehöriger</t>
+  </si>
+  <si>
+    <t>Unzufriedenheit mit der beruflichen Zeitverwendung</t>
+  </si>
+  <si>
+    <t>Unzufriedenheit mit der Zeitverwendung für die Hausarbeit</t>
+  </si>
+  <si>
+    <t>Unzufriedenheit mit der aufgewendeten Zeit für die  Angehörigen</t>
+  </si>
+  <si>
+    <t>Unzufriedenheit mit der aufgewendeten Zeit für die Partnerschaft</t>
+  </si>
+  <si>
+    <t>Unzufriedenheit mit der Qualität der Zeit für die Partnerschaft</t>
+  </si>
+  <si>
+    <t>Unzufriedenheit mit aufgewendeter Zeit für Freizeit</t>
+  </si>
+  <si>
+    <t>Unzufriedenheit mit aufgewendeter Zeit für sozialen Beziehungen</t>
+  </si>
+  <si>
+    <t>Unzufriedenheiten: Mangelnde Wertschätzung</t>
+  </si>
+  <si>
+    <t>Unzufriedenheiten: Lohn</t>
+  </si>
+  <si>
+    <t>Belastung: Zu viele Dinge zu erledigen in der Freizeit</t>
+  </si>
+  <si>
+    <t>Belastung: Hoher Zeitdruck bei der Arbeit</t>
+  </si>
+  <si>
+    <t>Belastung: Erwartungen Arbeitgeber/Kollegen</t>
+  </si>
+  <si>
+    <t>Belastung: Eigene Erwartungen an Hausarbeit/Betreuung von Angehörigen nicht erfüllen können </t>
   </si>
 </sst>
 </file>
@@ -533,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -543,6 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1068,27 +1081,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F2727F-E159-4B39-B30A-A10ACC8F5533}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="117" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" customWidth="1"/>
-    <col min="9" max="9" width="41.83203125" customWidth="1"/>
-    <col min="10" max="10" width="70.5" customWidth="1"/>
-    <col min="11" max="12" width="10.83203125" customWidth="1"/>
-    <col min="13" max="13" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="41.85546875" customWidth="1"/>
+    <col min="10" max="10" width="70.42578125" customWidth="1"/>
+    <col min="11" max="12" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1096,22 +1109,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -1126,1036 +1139,1020 @@
         <v>9</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="K2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="8"/>
-      <c r="I3" s="5" t="s">
-        <v>13</v>
+      <c r="I3" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="8"/>
-      <c r="I5" s="5" t="s">
-        <v>17</v>
+      <c r="I5" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" s="8"/>
-      <c r="I6" s="5" t="s">
-        <v>17</v>
+      <c r="I6" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="8"/>
-      <c r="I7" s="5" t="s">
-        <v>19</v>
+      <c r="I7" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="8"/>
-      <c r="I8" s="5" t="s">
-        <v>19</v>
+      <c r="I8" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="8"/>
       <c r="I12" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="5" t="s">
-        <v>105</v>
+      <c r="I13" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="5" t="s">
-        <v>107</v>
+      <c r="I14" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H15" s="8"/>
-      <c r="I15" s="5" t="s">
-        <v>21</v>
+      <c r="I15" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" s="8"/>
-      <c r="I16" s="5" t="s">
-        <v>22</v>
+      <c r="I16" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="8"/>
-      <c r="I17" s="5" t="s">
-        <v>25</v>
+      <c r="I17" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="5" t="s">
-        <v>26</v>
+      <c r="I18" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19" s="8"/>
-      <c r="I19" s="5" t="s">
-        <v>26</v>
+      <c r="I19" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20" s="8"/>
-      <c r="I20" s="5" t="s">
-        <v>25</v>
+      <c r="I20" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G23" s="3"/>
       <c r="H23" s="8"/>
       <c r="I23" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
       <c r="M23" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="3" t="s">
-        <v>121</v>
+      <c r="B24" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="5" t="s">
-        <v>29</v>
+      <c r="I24" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
-      <c r="M24" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M24" s="9"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G25" s="3"/>
       <c r="H25" s="8"/>
       <c r="I25" s="5" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="9"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H27" s="8"/>
-      <c r="I27" s="5" t="s">
-        <v>110</v>
+      <c r="I27" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H28" s="8"/>
-      <c r="I28" s="5" t="s">
-        <v>31</v>
+      <c r="I28" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H29" s="8"/>
-      <c r="I29" s="5" t="s">
-        <v>32</v>
+      <c r="I29" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H30" s="8"/>
-      <c r="I30" s="5" t="s">
-        <v>33</v>
+      <c r="I30" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2171,19 +2168,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B49719-3F28-457B-AF20-CD1813ACC6B3}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="190.5" customWidth="1"/>
-    <col min="3" max="3" width="68.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="190.42578125" customWidth="1"/>
+    <col min="3" max="3" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2191,178 +2188,178 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3.1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.0999999999999996</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4.2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.0999999999999996</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5.2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6.1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6.2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2381,13 +2378,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2395,55 +2392,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
   </sheetData>
@@ -2458,21 +2455,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E396E85-B3B1-449F-B640-6DB26BD002CF}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="118" customWidth="1"/>
-    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="81.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="71.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2480,201 +2477,201 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adaption of gap_types to 2 groups ("Arbeit" & "Privat") instead of 3 groups ("Arbeit", "Soziales Umfeld", "Hausarbeit & Selbstsorge"). -> Adapted Excels, New Testcases (old testcases deleted), New graphics in Zwischenauswertung.
</commit_message>
<xml_diff>
--- a/inst/shiny-apps/vsim/data/vsim_question_lists_aeltere_arbeitnehmende.xlsx
+++ b/inst/shiny-apps/vsim/data/vsim_question_lists_aeltere_arbeitnehmende.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAY\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SLC\Desktop\IMS\packages\vsim\inst\shiny-apps\vsim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95703483-9EE1-42FA-83BF-D5DF9ABC0B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21ED098E-70B2-4D0E-B360-759336C41490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
   </bookViews>
   <sheets>
     <sheet name="QAGlist_Teil1" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="145">
   <si>
     <t>Qnum</t>
   </si>
@@ -344,15 +344,6 @@
     <t>Arbeit</t>
   </si>
   <si>
-    <t>Haushalt &amp; Selbstsorge</t>
-  </si>
-  <si>
-    <t>Soziales Umfeld</t>
-  </si>
-  <si>
-    <t>Arbeit,Haushalt &amp; Selbstsorge</t>
-  </si>
-  <si>
     <t>Ich bin zufrieden mit meinen aktuellen Möglichkeiten zur Karriereentwicklung.</t>
   </si>
   <si>
@@ -377,9 +368,6 @@
     <t>Ich fühle mich belastet, weil es mir emotional oft nicht gut geht.</t>
   </si>
   <si>
-    <t>Arbeit, Haushalt &amp; Selbstsorge</t>
-  </si>
-  <si>
     <t>Finden Sie es in Ordnung, wie viel Zeit Sie pro Woche für die Erwerbsarbeit (inkl. Pendeln, Übernachtungen, Pausen und Mittagszeiten) aufwenden?</t>
   </si>
   <si>
@@ -480,6 +468,12 @@
   </si>
   <si>
     <t>Belastung: Eigene Erwartungen an Hausarbeit/Betreuung von Angehörigen nicht erfüllen können </t>
+  </si>
+  <si>
+    <t>Privat</t>
+  </si>
+  <si>
+    <t>Arbeit, Privat</t>
   </si>
 </sst>
 </file>
@@ -1081,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F2727F-E159-4B39-B30A-A10ACC8F5533}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1139,7 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>57</v>
@@ -1160,7 +1154,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="8"/>
       <c r="I2" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>10</v>
@@ -1178,7 +1172,7 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>57</v>
@@ -1195,7 +1189,7 @@
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>10</v>
@@ -1207,13 +1201,13 @@
         <v>11</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>57</v>
@@ -1230,7 +1224,7 @@
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>10</v>
@@ -1242,7 +1236,7 @@
         <v>11</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1267,7 +1261,7 @@
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>15</v>
@@ -1279,7 +1273,7 @@
         <v>11</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1304,7 +1298,7 @@
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>15</v>
@@ -1316,7 +1310,7 @@
         <v>11</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1341,7 +1335,7 @@
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>15</v>
@@ -1353,7 +1347,7 @@
         <v>11</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1378,7 +1372,7 @@
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>15</v>
@@ -1390,13 +1384,13 @@
         <v>11</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>91</v>
@@ -1462,7 +1456,7 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>91</v>
@@ -1526,7 +1520,7 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>61</v>
@@ -1543,7 +1537,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="8"/>
       <c r="I13" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>15</v>
@@ -1574,7 +1568,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="8"/>
       <c r="I14" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>15</v>
@@ -1588,7 +1582,7 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>61</v>
@@ -1662,7 +1656,7 @@
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>61</v>
@@ -1681,7 +1675,7 @@
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>20</v>
@@ -1693,7 +1687,7 @@
         <v>11</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1718,7 +1712,7 @@
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>20</v>
@@ -1736,7 +1730,7 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>61</v>
@@ -1755,7 +1749,7 @@
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>20</v>
@@ -1773,7 +1767,7 @@
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>61</v>
@@ -1792,7 +1786,7 @@
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>20</v>
@@ -1804,13 +1798,13 @@
         <v>11</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>61</v>
@@ -1841,13 +1835,13 @@
         <v>11</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>61</v>
@@ -1878,13 +1872,13 @@
         <v>11</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>61</v>
@@ -1909,13 +1903,13 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="6" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>61</v>
@@ -1932,7 +1926,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="8"/>
       <c r="I24" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>20</v>
@@ -1944,7 +1938,7 @@
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>61</v>
@@ -1961,7 +1955,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="8"/>
       <c r="I25" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>20</v>
@@ -1973,7 +1967,7 @@
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>61</v>
@@ -1992,7 +1986,7 @@
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>20</v>
@@ -2004,7 +1998,7 @@
         <v>11</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2047,7 +2041,7 @@
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>61</v>
@@ -2078,13 +2072,13 @@
         <v>11</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>61</v>
@@ -2103,7 +2097,7 @@
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>20</v>
@@ -2115,13 +2109,13 @@
         <v>11</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>61</v>
@@ -2140,7 +2134,7 @@
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>20</v>
@@ -2152,7 +2146,7 @@
         <v>11</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2413,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2520,16 +2514,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>70</v>
@@ -2543,16 +2537,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">

</xml_diff>